<commit_message>
Simulated Combined Input Impedance Calculated
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ugsamba\cm21g15\D3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominicheaton/Library/Mobile Documents/com~apple~CloudDocs/Soton/2nd Year/Labs/D__/D3/D3/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="25520" windowHeight="15560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
   <si>
     <t>CE Amp</t>
   </si>
@@ -148,16 +154,19 @@
   <si>
     <t>With Ce Bypassing Re1 and Re2</t>
   </si>
+  <si>
+    <t>Simulated Input Imp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
-    <numFmt numFmtId="169" formatCode="0.00000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -228,8 +237,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -252,7 +261,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -366,76 +375,76 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5000</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10000</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20000</c:v>
+                  <c:v>20000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50000</c:v>
+                  <c:v>50000.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>100000</c:v>
+                  <c:v>100000.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>200000</c:v>
+                  <c:v>200000.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>500000</c:v>
+                  <c:v>500000.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1000000</c:v>
+                  <c:v>1.0E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2000000</c:v>
+                  <c:v>2.0E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5000000</c:v>
+                  <c:v>5.0E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10000000</c:v>
+                  <c:v>1.0E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20000000</c:v>
+                  <c:v>2.0E7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>50000000</c:v>
+                  <c:v>5.0E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -450,19 +459,19 @@
                   <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36299999999999999</c:v>
+                  <c:v>0.363</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85299999999999998</c:v>
+                  <c:v>0.853</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1.649</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9670000000000001</c:v>
+                  <c:v>2.967</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.6559999999999997</c:v>
+                  <c:v>4.656</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5.36</c:v>
@@ -477,16 +486,16 @@
                   <c:v>5.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.8869999999999996</c:v>
+                  <c:v>5.887</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.7359999999999998</c:v>
+                  <c:v>5.736</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.5759999999999996</c:v>
+                  <c:v>5.576</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.3920000000000003</c:v>
+                  <c:v>5.392</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5.37</c:v>
@@ -507,13 +516,13 @@
                   <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>4.4</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>2.2</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>1.3</c:v>
@@ -522,7 +531,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1E58-4DA8-99F9-98A79B7BF9F4}"/>
             </c:ext>
@@ -536,13 +545,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1667986031"/>
-        <c:axId val="1667986863"/>
+        <c:axId val="1285776576"/>
+        <c:axId val="1285778896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1667986031"/>
+        <c:axId val="1285776576"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -598,12 +607,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1667986863"/>
+        <c:crossAx val="1285778896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1667986863"/>
+        <c:axId val="1285778896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,7 +669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1667986031"/>
+        <c:crossAx val="1285776576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -710,7 +719,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -827,73 +836,73 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5000</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10000</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20000</c:v>
+                  <c:v>20000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50000</c:v>
+                  <c:v>50000.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>100000</c:v>
+                  <c:v>100000.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>200000</c:v>
+                  <c:v>200000.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>500000</c:v>
+                  <c:v>500000.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1000000</c:v>
+                  <c:v>1.0E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2000000</c:v>
+                  <c:v>2.0E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5000000</c:v>
+                  <c:v>5.0E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10000000</c:v>
+                  <c:v>1.0E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20000000</c:v>
+                  <c:v>2.0E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -908,76 +917,76 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54166666666666674</c:v>
+                  <c:v>0.541666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70833333333333337</c:v>
+                  <c:v>0.708333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.83333333333333337</c:v>
+                  <c:v>0.833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.93750000000000011</c:v>
+                  <c:v>0.9375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0020833333333334</c:v>
+                  <c:v>1.002083333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0072916666666667</c:v>
+                  <c:v>1.007291666666667</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.003125</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0208333333333333</c:v>
+                  <c:v>1.020833333333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0322916666666666</c:v>
+                  <c:v>1.032291666666667</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0239583333333333</c:v>
+                  <c:v>1.023958333333333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0140237324703343</c:v>
+                  <c:v>1.014023732470334</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.0454545454545454</c:v>
+                  <c:v>1.045454545454545</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.0169491525423728</c:v>
+                  <c:v>1.016949152542373</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0476190476190477</c:v>
+                  <c:v>1.047619047619048</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.0476190476190477</c:v>
+                  <c:v>1.047619047619048</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.0227272727272727</c:v>
+                  <c:v>1.022727272727273</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0227272727272727</c:v>
+                  <c:v>1.022727272727273</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.0227272727272727</c:v>
+                  <c:v>1.022727272727273</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0227272727272727</c:v>
+                  <c:v>1.022727272727273</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.0227272727272727</c:v>
+                  <c:v>1.022727272727273</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.0526315789473684</c:v>
+                  <c:v>1.052631578947368</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.0555555555555554</c:v>
+                  <c:v>1.055555555555555</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-BF69-4113-AB9D-148D6C66998B}"/>
             </c:ext>
@@ -991,13 +1000,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1694062959"/>
-        <c:axId val="1694067951"/>
+        <c:axId val="1285801664"/>
+        <c:axId val="1285804144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1694062959"/>
+        <c:axId val="1285801664"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1053,12 +1062,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1694067951"/>
+        <c:crossAx val="1285804144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1694067951"/>
+        <c:axId val="1285804144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1115,7 +1124,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1694062959"/>
+        <c:crossAx val="1285801664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1165,7 +1174,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1279,73 +1288,73 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5000</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10000</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20000</c:v>
+                  <c:v>20000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50000</c:v>
+                  <c:v>50000.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>100000</c:v>
+                  <c:v>100000.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>200000</c:v>
+                  <c:v>200000.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>500000</c:v>
+                  <c:v>500000.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1000000</c:v>
+                  <c:v>1.0E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2000000</c:v>
+                  <c:v>2.0E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5000000</c:v>
+                  <c:v>5.0E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10000000</c:v>
+                  <c:v>1.0E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20000000</c:v>
+                  <c:v>2.0E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1357,46 +1366,46 @@
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>3.8999999999999993E-2</c:v>
+                  <c:v>0.039</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16750000000000001</c:v>
+                  <c:v>0.1675</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.63180341186027622</c:v>
+                  <c:v>0.631803411860276</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4313111941051782</c:v>
+                  <c:v>1.431311194105178</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6732878129526174</c:v>
+                  <c:v>2.673287812952617</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.325051759834369</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.108628181253879</c:v>
+                  <c:v>5.108628181253878</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.3933747412008284</c:v>
+                  <c:v>5.393374741200828</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.4192436378383855</c:v>
+                  <c:v>5.419243637838385</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.4214539908490087</c:v>
+                  <c:v>5.421453990849008</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.4926210766992307</c:v>
+                  <c:v>5.492621076699231</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.5037194473963877</c:v>
+                  <c:v>5.503719447396388</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.4777415852334412</c:v>
+                  <c:v>5.47774158523344</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.4666666666666668</c:v>
+                  <c:v>5.466666666666666</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5.5</c:v>
@@ -1405,31 +1414,31 @@
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.5111111111111111</c:v>
+                  <c:v>5.511111111111111</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.4666666666666668</c:v>
+                  <c:v>5.466666666666666</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>5.406593406593406</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.1739130434782608</c:v>
+                  <c:v>5.173913043478261</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.4888888888888889</c:v>
+                  <c:v>4.488888888888889</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.1515151515151514</c:v>
+                  <c:v>3.151515151515151</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.6956521739130435</c:v>
+                  <c:v>1.695652173913043</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-1BDE-451B-B0BD-2392613B103F}"/>
             </c:ext>
@@ -1443,13 +1452,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1704741887"/>
-        <c:axId val="1704740639"/>
+        <c:axId val="1284640432"/>
+        <c:axId val="1284642480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1704741887"/>
+        <c:axId val="1284640432"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1505,12 +1514,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1704740639"/>
+        <c:crossAx val="1284642480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1704740639"/>
+        <c:axId val="1284642480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1567,7 +1576,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1704741887"/>
+        <c:crossAx val="1284640432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1617,7 +1626,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1726,73 +1735,73 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5000</c:v>
+                  <c:v>5000.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10000</c:v>
+                  <c:v>10000.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20000</c:v>
+                  <c:v>20000.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50000</c:v>
+                  <c:v>50000.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>100000</c:v>
+                  <c:v>100000.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>200000</c:v>
+                  <c:v>200000.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>500000</c:v>
+                  <c:v>500000.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1000000</c:v>
+                  <c:v>1.0E6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2000000</c:v>
+                  <c:v>2.0E6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5000000</c:v>
+                  <c:v>5.0E6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10000000</c:v>
+                  <c:v>1.0E7</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20000000</c:v>
+                  <c:v>2.0E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1804,79 +1813,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>2.9666254635352281E-3</c:v>
+                  <c:v>0.00296662546353523</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.597402597402597E-3</c:v>
+                  <c:v>0.0025974025974026</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3397761953204478E-3</c:v>
+                  <c:v>0.00233977619532045</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.4291497975708499E-3</c:v>
+                  <c:v>0.00242914979757085</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1055900621118015E-3</c:v>
+                  <c:v>0.0031055900621118</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1055900621118015E-3</c:v>
+                  <c:v>0.0031055900621118</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2091097308488614E-3</c:v>
+                  <c:v>0.00320910973084886</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.1055900621118015E-3</c:v>
+                  <c:v>0.0031055900621118</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.6585365853658534E-3</c:v>
+                  <c:v>0.00365853658536585</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.6622583926754831E-3</c:v>
+                  <c:v>0.00366225839267548</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.1580041580041582E-3</c:v>
+                  <c:v>0.00415800415800416</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.4565217391304346E-3</c:v>
+                  <c:v>0.00445652173913043</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.043478260869565E-2</c:v>
+                  <c:v>0.0304347826086956</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.1818181818181822E-2</c:v>
+                  <c:v>0.0318181818181818</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.5227272727272725E-2</c:v>
+                  <c:v>0.0352272727272727</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.8636363636363642E-2</c:v>
+                  <c:v>0.0386363636363636</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.333333333333333E-2</c:v>
+                  <c:v>0.0533333333333333</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.10111111111111111</c:v>
+                  <c:v>0.101111111111111</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.27727272727272728</c:v>
+                  <c:v>0.277272727272727</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.48444444444444446</c:v>
+                  <c:v>0.484444444444444</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.57872340425531921</c:v>
+                  <c:v>0.578723404255319</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.62499999999999989</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-5C43-4A16-AC46-C7625E6AF623}"/>
             </c:ext>
@@ -1890,13 +1899,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1704744383"/>
-        <c:axId val="1704742303"/>
+        <c:axId val="1284664176"/>
+        <c:axId val="1284666656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1704744383"/>
+        <c:axId val="1284664176"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1952,12 +1961,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1704742303"/>
+        <c:crossAx val="1284666656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1704742303"/>
+        <c:axId val="1284666656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2014,7 +2023,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1704744383"/>
+        <c:crossAx val="1284664176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4809,25 +4818,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="D136" sqref="D136"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="22" max="22" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
+    <col min="22" max="22" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -4841,7 +4851,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>1</v>
       </c>
@@ -4856,7 +4866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -4867,7 +4877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>1</v>
       </c>
@@ -4879,7 +4889,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>2</v>
       </c>
@@ -4891,7 +4901,7 @@
         <v>0.36299999999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>5</v>
       </c>
@@ -4903,7 +4913,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>10</v>
       </c>
@@ -4915,7 +4925,7 @@
         <v>1.649</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>20</v>
       </c>
@@ -4927,7 +4937,7 @@
         <v>2.9670000000000001</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>50</v>
       </c>
@@ -4939,7 +4949,7 @@
         <v>4.6559999999999997</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>100</v>
       </c>
@@ -4954,7 +4964,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>200</v>
       </c>
@@ -4975,7 +4985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>500</v>
       </c>
@@ -4997,7 +5007,7 @@
         <v>5.3581011351909185</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>1000</v>
       </c>
@@ -5009,7 +5019,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>2000</v>
       </c>
@@ -5021,7 +5031,7 @@
         <v>5.8869999999999996</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>5000</v>
       </c>
@@ -5036,7 +5046,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>10000</v>
       </c>
@@ -5057,7 +5067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>20000</v>
       </c>
@@ -5079,7 +5089,7 @@
         <v>95.833333333333343</v>
       </c>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>50000</v>
       </c>
@@ -5091,7 +5101,7 @@
         <v>5.37</v>
       </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>100000</v>
       </c>
@@ -5103,7 +5113,7 @@
         <v>5.36</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <v>200000</v>
       </c>
@@ -5115,7 +5125,7 @@
         <v>5.44</v>
       </c>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <v>500000</v>
       </c>
@@ -5127,7 +5137,7 @@
         <v>5.44</v>
       </c>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
         <v>1000000</v>
       </c>
@@ -5139,7 +5149,7 @@
         <v>5.36</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
         <v>2000000</v>
       </c>
@@ -5151,7 +5161,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
         <v>5000000</v>
       </c>
@@ -5163,7 +5173,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
         <v>10000000</v>
       </c>
@@ -5175,7 +5185,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <v>20000000</v>
       </c>
@@ -5187,7 +5197,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B31" s="1">
         <v>50000000</v>
       </c>
@@ -5199,7 +5209,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
         <v>10</v>
       </c>
@@ -5207,7 +5217,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>11</v>
       </c>
@@ -5215,7 +5225,7 @@
         <v>1.15438</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>13</v>
       </c>
@@ -5223,7 +5233,7 @@
         <v>7.1355000000000004</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>14</v>
       </c>
@@ -5231,7 +5241,7 @@
         <v>0.50355000000000005</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>15</v>
       </c>
@@ -5239,7 +5249,7 @@
         <v>7.3200000000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
         <v>6</v>
       </c>
@@ -5248,7 +5258,7 @@
         <v>54.959k</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>18</v>
       </c>
@@ -5259,7 +5269,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>19</v>
       </c>
@@ -5271,7 +5281,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>20</v>
       </c>
@@ -5279,7 +5289,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F43" t="s">
         <v>38</v>
       </c>
@@ -5287,7 +5297,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
         <v>7</v>
       </c>
@@ -5305,7 +5315,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E45" t="s">
         <v>32</v>
       </c>
@@ -5316,7 +5326,7 @@
         <v>7.16</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E46" t="s">
         <v>33</v>
       </c>
@@ -5327,7 +5337,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E47" t="s">
         <v>34</v>
       </c>
@@ -5340,7 +5350,7 @@
         <v>2135.5932203389825</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -5359,12 +5369,12 @@
       <c r="P49" s="4"/>
       <c r="Q49" s="4"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B51" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>4</v>
       </c>
@@ -5381,7 +5391,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B54">
         <v>0.96</v>
       </c>
@@ -5396,7 +5406,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>8</v>
       </c>
@@ -5407,7 +5417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B57" s="1">
         <v>1</v>
       </c>
@@ -5419,7 +5429,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B58" s="1">
         <v>2</v>
       </c>
@@ -5431,7 +5441,7 @@
         <v>0.54166666666666674</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B59" s="1">
         <v>5</v>
       </c>
@@ -5443,7 +5453,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B60" s="1">
         <v>10</v>
       </c>
@@ -5455,7 +5465,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B61" s="1">
         <v>20</v>
       </c>
@@ -5467,7 +5477,7 @@
         <v>0.93750000000000011</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B62" s="1">
         <v>50</v>
       </c>
@@ -5479,7 +5489,7 @@
         <v>1.0020833333333334</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B63" s="1">
         <v>100</v>
       </c>
@@ -5491,7 +5501,7 @@
         <v>1.0072916666666667</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B64" s="1">
         <v>200</v>
       </c>
@@ -5503,7 +5513,7 @@
         <v>1.003125</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="1">
         <v>500</v>
       </c>
@@ -5515,7 +5525,7 @@
         <v>1.0208333333333333</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" s="1">
         <v>1000</v>
       </c>
@@ -5527,7 +5537,7 @@
         <v>1.0322916666666666</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" s="1">
         <v>2000</v>
       </c>
@@ -5539,7 +5549,7 @@
         <v>1.0239583333333333</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B68" s="1">
         <v>5000</v>
       </c>
@@ -5551,7 +5561,7 @@
         <v>1.0140237324703343</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B69" s="1">
         <v>10000</v>
       </c>
@@ -5563,7 +5573,7 @@
         <v>1.0454545454545454</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B70" s="1">
         <v>20000</v>
       </c>
@@ -5575,7 +5585,7 @@
         <v>1.0169491525423728</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B71" s="1">
         <v>50000</v>
       </c>
@@ -5587,7 +5597,7 @@
         <v>1.0476190476190477</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B72" s="1">
         <v>100000</v>
       </c>
@@ -5599,7 +5609,7 @@
         <v>1.0476190476190477</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73" s="1">
         <v>200000</v>
       </c>
@@ -5611,7 +5621,7 @@
         <v>1.0227272727272727</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B74" s="1">
         <v>500000</v>
       </c>
@@ -5623,7 +5633,7 @@
         <v>1.0227272727272727</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B75" s="1">
         <v>1000000</v>
       </c>
@@ -5635,7 +5645,7 @@
         <v>1.0227272727272727</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B76" s="1">
         <v>2000000</v>
       </c>
@@ -5647,7 +5657,7 @@
         <v>1.0227272727272727</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B77" s="1">
         <v>5000000</v>
       </c>
@@ -5659,7 +5669,7 @@
         <v>1.0227272727272727</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B78" s="1">
         <v>10000000</v>
       </c>
@@ -5671,7 +5681,7 @@
         <v>1.0526315789473684</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B79" s="1">
         <v>20000000</v>
       </c>
@@ -5683,7 +5693,7 @@
         <v>1.0555555555555554</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>8</v>
       </c>
@@ -5697,7 +5707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B83" s="1">
         <v>1</v>
       </c>
@@ -5712,7 +5722,7 @@
         <v>2.9666254635352281E-3</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B84" s="1">
         <v>2</v>
       </c>
@@ -5727,7 +5737,7 @@
         <v>2.597402597402597E-3</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B85" s="1">
         <v>5</v>
       </c>
@@ -5742,7 +5752,7 @@
         <v>2.3397761953204478E-3</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B86" s="1">
         <v>10</v>
       </c>
@@ -5757,7 +5767,7 @@
         <v>2.4291497975708499E-3</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B87" s="1">
         <v>20</v>
       </c>
@@ -5772,7 +5782,7 @@
         <v>3.1055900621118015E-3</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B88" s="1">
         <v>50</v>
       </c>
@@ -5787,7 +5797,7 @@
         <v>3.1055900621118015E-3</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B89" s="1">
         <v>100</v>
       </c>
@@ -5802,7 +5812,7 @@
         <v>3.2091097308488614E-3</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B90" s="1">
         <v>200</v>
       </c>
@@ -5817,7 +5827,7 @@
         <v>3.1055900621118015E-3</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B91" s="1">
         <v>500</v>
       </c>
@@ -5832,7 +5842,7 @@
         <v>3.6585365853658534E-3</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B92" s="1">
         <v>1000</v>
       </c>
@@ -5847,7 +5857,7 @@
         <v>3.6622583926754831E-3</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B93" s="1">
         <v>2000</v>
       </c>
@@ -5862,7 +5872,7 @@
         <v>4.1580041580041582E-3</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B94" s="1">
         <v>5000</v>
       </c>
@@ -5877,7 +5887,7 @@
         <v>4.4565217391304346E-3</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B95" s="1">
         <v>10000</v>
       </c>
@@ -5892,7 +5902,7 @@
         <v>3.043478260869565E-2</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B96" s="1">
         <v>20000</v>
       </c>
@@ -5907,7 +5917,7 @@
         <v>3.1818181818181822E-2</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B97" s="1">
         <v>50000</v>
       </c>
@@ -5922,7 +5932,7 @@
         <v>3.5227272727272725E-2</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B98" s="1">
         <v>100000</v>
       </c>
@@ -5937,7 +5947,7 @@
         <v>3.8636363636363642E-2</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B99" s="1">
         <v>200000</v>
       </c>
@@ -5952,7 +5962,7 @@
         <v>5.333333333333333E-2</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B100" s="1">
         <v>500000</v>
       </c>
@@ -5967,7 +5977,7 @@
         <v>0.10111111111111111</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B101" s="1">
         <v>1000000</v>
       </c>
@@ -5982,7 +5992,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B102" s="1">
         <v>2000000</v>
       </c>
@@ -5997,7 +6007,7 @@
         <v>0.27727272727272728</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B103" s="1">
         <v>5000000</v>
       </c>
@@ -6012,7 +6022,7 @@
         <v>0.48444444444444446</v>
       </c>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B104" s="1">
         <v>10000000</v>
       </c>
@@ -6027,7 +6037,7 @@
         <v>0.57872340425531921</v>
       </c>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B105" s="1">
         <v>20000000</v>
       </c>
@@ -6042,7 +6052,7 @@
         <v>0.62499999999999989</v>
       </c>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B107" s="3" t="s">
         <v>10</v>
       </c>
@@ -6050,7 +6060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>22</v>
       </c>
@@ -6058,7 +6068,7 @@
         <v>5.2965999999999998</v>
       </c>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>23</v>
       </c>
@@ -6066,7 +6076,7 @@
         <v>4.6509499999999999</v>
       </c>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B111" s="3" t="s">
         <v>6</v>
       </c>
@@ -6075,7 +6085,7 @@
         <v>24456.356127729108</v>
       </c>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B112" s="5" t="s">
         <v>27</v>
       </c>
@@ -6083,7 +6093,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>25</v>
       </c>
@@ -6091,7 +6101,7 @@
         <v>0.35299999999999998</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>26</v>
       </c>
@@ -6099,7 +6109,7 @@
         <v>8.4270000000000005E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>28</v>
       </c>
@@ -6111,7 +6121,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>29</v>
       </c>
@@ -6123,7 +6133,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>20</v>
       </c>
@@ -6132,7 +6142,7 @@
         <v>24456.356127729108</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="F118" t="s">
         <v>38</v>
       </c>
@@ -6140,7 +6150,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B119" s="3" t="s">
         <v>7</v>
       </c>
@@ -6158,7 +6168,7 @@
         <v>4.5847499999999997</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E120" t="s">
         <v>32</v>
       </c>
@@ -6169,7 +6179,7 @@
         <v>4.6276599999999997</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E121" t="s">
         <v>33</v>
       </c>
@@ -6180,7 +6190,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E122" t="s">
         <v>34</v>
       </c>
@@ -6193,7 +6203,7 @@
         <v>93.592889470527297</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -6212,12 +6222,12 @@
       <c r="P124" s="4"/>
       <c r="Q124" s="4"/>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B126" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>4</v>
       </c>
@@ -6231,7 +6241,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B129">
         <v>0.98499999999999999</v>
       </c>
@@ -6246,7 +6256,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B131" s="3" t="s">
         <v>6</v>
       </c>
@@ -6255,31 +6265,40 @@
         <v>46258.604100362674</v>
       </c>
     </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B132" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C132">
         <v>1000000</v>
       </c>
-    </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F132" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>25</v>
       </c>
       <c r="C133" s="2">
         <v>0.35339999999999999</v>
       </c>
-    </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F133" s="9">
+        <v>0.35299999999999998</v>
+      </c>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>26</v>
       </c>
       <c r="C134">
         <v>1.5625E-2</v>
       </c>
-    </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F134" s="9">
+        <v>0.29299999999999998</v>
+      </c>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>28</v>
       </c>
@@ -6287,8 +6306,12 @@
         <f>C133-C134</f>
         <v>0.33777499999999999</v>
       </c>
-    </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F135" s="9">
+        <f>F133-F134</f>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>29</v>
       </c>
@@ -6296,8 +6319,12 @@
         <f>C135/C132</f>
         <v>3.3777499999999997E-7</v>
       </c>
-    </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F136" s="9">
+        <f>F135/10000</f>
+        <v>6.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>20</v>
       </c>
@@ -6305,8 +6332,12 @@
         <f>C134/C136</f>
         <v>46258.604100362674</v>
       </c>
-    </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F137" s="9">
+        <f>F134/F136</f>
+        <v>48833.333333333328</v>
+      </c>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F138" t="s">
         <v>38</v>
       </c>
@@ -6314,7 +6345,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B139" s="3" t="s">
         <v>7</v>
       </c>
@@ -6332,7 +6363,7 @@
         <v>4.58</v>
       </c>
     </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E140" t="s">
         <v>32</v>
       </c>
@@ -6343,7 +6374,7 @@
         <v>4.63</v>
       </c>
     </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E141" t="s">
         <v>33</v>
       </c>
@@ -6354,7 +6385,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
       <c r="E142" t="s">
         <v>34</v>
       </c>
@@ -6367,7 +6398,7 @@
         <v>109.17030567685551</v>
       </c>
     </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>8</v>
       </c>
@@ -6381,7 +6412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B145" s="1">
         <v>1</v>
       </c>
@@ -6396,7 +6427,7 @@
         <v>3.8999999999999993E-2</v>
       </c>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B146" s="1">
         <v>2</v>
       </c>
@@ -6411,7 +6442,7 @@
         <v>0.16750000000000001</v>
       </c>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B147" s="1">
         <v>5</v>
       </c>
@@ -6426,7 +6457,7 @@
         <v>0.63180341186027622</v>
       </c>
     </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B148" s="1">
         <v>10</v>
       </c>
@@ -6441,7 +6472,7 @@
         <v>1.4313111941051782</v>
       </c>
     </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B149" s="1">
         <v>20</v>
       </c>
@@ -6456,7 +6487,7 @@
         <v>2.6732878129526174</v>
       </c>
     </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B150" s="1">
         <v>50</v>
       </c>
@@ -6471,7 +6502,7 @@
         <v>4.325051759834369</v>
       </c>
     </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B151" s="1">
         <v>100</v>
       </c>
@@ -6486,7 +6517,7 @@
         <v>5.108628181253879</v>
       </c>
     </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B152" s="1">
         <v>200</v>
       </c>
@@ -6501,7 +6532,7 @@
         <v>5.3933747412008284</v>
       </c>
     </row>
-    <row r="153" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B153" s="1">
         <v>500</v>
       </c>
@@ -6516,7 +6547,7 @@
         <v>5.4192436378383855</v>
       </c>
     </row>
-    <row r="154" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B154" s="1">
         <v>1000</v>
       </c>
@@ -6531,7 +6562,7 @@
         <v>5.4214539908490087</v>
       </c>
     </row>
-    <row r="155" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B155" s="1">
         <v>2000</v>
       </c>
@@ -6546,7 +6577,7 @@
         <v>5.4926210766992307</v>
       </c>
     </row>
-    <row r="156" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B156" s="1">
         <v>5000</v>
       </c>
@@ -6561,7 +6592,7 @@
         <v>5.5037194473963877</v>
       </c>
     </row>
-    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B157" s="1">
         <v>10000</v>
       </c>
@@ -6576,7 +6607,7 @@
         <v>5.4777415852334412</v>
       </c>
     </row>
-    <row r="158" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B158" s="1">
         <v>20000</v>
       </c>
@@ -6591,7 +6622,7 @@
         <v>5.4666666666666668</v>
       </c>
     </row>
-    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B159" s="1">
         <v>50000</v>
       </c>
@@ -6606,7 +6637,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="160" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B160" s="1">
         <v>100000</v>
       </c>
@@ -6621,7 +6652,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B161" s="1">
         <v>200000</v>
       </c>
@@ -6636,7 +6667,7 @@
         <v>5.5111111111111111</v>
       </c>
     </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B162" s="1">
         <v>500000</v>
       </c>
@@ -6651,7 +6682,7 @@
         <v>5.4666666666666668</v>
       </c>
     </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B163" s="1">
         <v>1000000</v>
       </c>
@@ -6666,7 +6697,7 @@
         <v>5.406593406593406</v>
       </c>
     </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B164" s="1">
         <v>2000000</v>
       </c>
@@ -6681,7 +6712,7 @@
         <v>5.1739130434782608</v>
       </c>
     </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B165" s="1">
         <v>5000000</v>
       </c>
@@ -6696,7 +6727,7 @@
         <v>4.4888888888888889</v>
       </c>
     </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B166" s="1">
         <v>10000000</v>
       </c>
@@ -6711,7 +6742,7 @@
         <v>3.1515151515151514</v>
       </c>
     </row>
-    <row r="167" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B167" s="1">
         <v>20000000</v>
       </c>

</xml_diff>

<commit_message>
WTF I made some changes apparently
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="25520" windowHeight="15560"/>
+    <workbookView xWindow="-25520" yWindow="-540" windowWidth="25520" windowHeight="15560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -305,7 +305,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -545,11 +544,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1285776576"/>
-        <c:axId val="1285778896"/>
+        <c:axId val="1285525232"/>
+        <c:axId val="1285527280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1285776576"/>
+        <c:axId val="1285525232"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -607,12 +606,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1285778896"/>
+        <c:crossAx val="1285527280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1285778896"/>
+        <c:axId val="1285527280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -669,7 +668,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1285776576"/>
+        <c:crossAx val="1285525232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -763,7 +762,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1000,11 +998,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1285801664"/>
-        <c:axId val="1285804144"/>
+        <c:axId val="1285511056"/>
+        <c:axId val="1285486784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1285801664"/>
+        <c:axId val="1285511056"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1062,12 +1060,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1285804144"/>
+        <c:crossAx val="1285486784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1285804144"/>
+        <c:axId val="1285486784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1124,7 +1122,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1285801664"/>
+        <c:crossAx val="1285511056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1452,11 +1450,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1284640432"/>
-        <c:axId val="1284642480"/>
+        <c:axId val="1317930704"/>
+        <c:axId val="1317932752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1284640432"/>
+        <c:axId val="1317930704"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1514,12 +1512,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1284642480"/>
+        <c:crossAx val="1317932752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1284642480"/>
+        <c:axId val="1317932752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1576,7 +1574,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1284640432"/>
+        <c:crossAx val="1317930704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1899,11 +1897,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1284664176"/>
-        <c:axId val="1284666656"/>
+        <c:axId val="1285393568"/>
+        <c:axId val="1284518704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1284664176"/>
+        <c:axId val="1285393568"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1961,12 +1959,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1284666656"/>
+        <c:crossAx val="1284518704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1284666656"/>
+        <c:axId val="1284518704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2023,7 +2021,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1284664176"/>
+        <c:crossAx val="1285393568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4818,8 +4816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="J119" sqref="J119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6165,7 +6163,7 @@
         <v>4.0806500000000003</v>
       </c>
       <c r="H119">
-        <v>4.5847499999999997</v>
+        <v>4.58</v>
       </c>
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.2">
@@ -6176,7 +6174,7 @@
         <v>4.1375400000000004</v>
       </c>
       <c r="H120">
-        <v>4.6276599999999997</v>
+        <v>4.6399999999999997</v>
       </c>
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.2">
@@ -6200,7 +6198,7 @@
       </c>
       <c r="H122">
         <f>(H121*(H120-H119))/H119</f>
-        <v>93.592889470527297</v>
+        <v>131.00436681222624</v>
       </c>
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>